<commit_message>
Updated ranking to include 'error' and 'not'
</commit_message>
<xml_diff>
--- a/ranking.xlsx
+++ b/ranking.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>AFF</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>DES</t>
+  </si>
+  <si>
+    <t>NOT</t>
+  </si>
+  <si>
+    <t>ERROR</t>
   </si>
 </sst>
 </file>
@@ -441,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,6 +680,19 @@
       </c>
       <c r="B28">
         <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>